<commit_message>
changed description for LED yellow, green and red
</commit_message>
<xml_diff>
--- a/Ventilator FI5 BOM Rev0.xlsx
+++ b/Ventilator FI5 BOM Rev0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://istitutoitalianotecnologia.sharepoint.com/sites/IITvsC19/Documenti condivisi/Repiratore/ferrari/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ventilator-fi5-mech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_815765C60015BCECD6925296FCD11D784FCA55A1" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176E0843-D13B-4060-A609-CB507B20612C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="23040" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="3540" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FI5-Rev0-Final" sheetId="1" r:id="rId1"/>
@@ -990,9 +990,6 @@
     <t xml:space="preserve">                VX-209491</t>
   </si>
   <si>
-    <t>LED YELLOW BIVAR MPR3HD</t>
-  </si>
-  <si>
     <t>LED3-LED6</t>
   </si>
   <si>
@@ -1008,9 +1005,6 @@
     <t xml:space="preserve">                VX-209493</t>
   </si>
   <si>
-    <t>LED GREEN BIVAR MPR3HD</t>
-  </si>
-  <si>
     <t>LED2</t>
   </si>
   <si>
@@ -1296,9 +1290,6 @@
     <t xml:space="preserve">                VX-209775</t>
   </si>
   <si>
-    <t>LED RED BIVAR MPR3HD</t>
-  </si>
-  <si>
     <t>LED1</t>
   </si>
   <si>
@@ -1345,6 +1336,15 @@
   </si>
   <si>
     <t>TRIMMED SIL CAP ID 10.3X25.4 ESSENTRA CODE 461704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED GREEN </t>
+  </si>
+  <si>
+    <t>LED YELLOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED RED </t>
   </si>
 </sst>
 </file>
@@ -1687,8 +1687,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H86" sqref="H86"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B163" sqref="B163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4244,7 +4244,7 @@
         <v>319</v>
       </c>
       <c r="B124" t="s">
-        <v>320</v>
+        <v>437</v>
       </c>
       <c r="C124" s="4">
         <v>0</v>
@@ -4253,76 +4253,76 @@
         <v>4</v>
       </c>
       <c r="E124" t="s">
+        <v>320</v>
+      </c>
+      <c r="F124" t="s">
         <v>321</v>
       </c>
-      <c r="F124" t="s">
+      <c r="G124" t="s">
         <v>322</v>
       </c>
-      <c r="G124" t="s">
+      <c r="H124" t="s">
         <v>323</v>
-      </c>
-      <c r="H124" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>324</v>
+      </c>
+      <c r="B125" t="s">
+        <v>436</v>
+      </c>
+      <c r="C125" s="4">
+        <v>0</v>
+      </c>
+      <c r="D125" s="5">
+        <v>1</v>
+      </c>
+      <c r="E125" t="s">
         <v>325</v>
       </c>
-      <c r="B125" t="s">
+      <c r="F125" t="s">
+        <v>321</v>
+      </c>
+      <c r="G125" t="s">
+        <v>322</v>
+      </c>
+      <c r="H125" t="s">
         <v>326</v>
-      </c>
-      <c r="C125" s="4">
-        <v>0</v>
-      </c>
-      <c r="D125" s="5">
-        <v>1</v>
-      </c>
-      <c r="E125" t="s">
-        <v>327</v>
-      </c>
-      <c r="F125" t="s">
-        <v>322</v>
-      </c>
-      <c r="G125" t="s">
-        <v>323</v>
-      </c>
-      <c r="H125" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
+        <v>327</v>
+      </c>
+      <c r="B126" t="s">
+        <v>328</v>
+      </c>
+      <c r="C126" s="4">
+        <v>0</v>
+      </c>
+      <c r="D126" s="5">
+        <v>1</v>
+      </c>
+      <c r="E126" t="s">
         <v>329</v>
-      </c>
-      <c r="B126" t="s">
-        <v>330</v>
-      </c>
-      <c r="C126" s="4">
-        <v>0</v>
-      </c>
-      <c r="D126" s="5">
-        <v>1</v>
-      </c>
-      <c r="E126" t="s">
-        <v>331</v>
       </c>
       <c r="F126" t="s">
         <v>143</v>
       </c>
       <c r="G126" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H126" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B127" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C127" s="4">
         <v>0</v>
@@ -4331,24 +4331,24 @@
         <v>2</v>
       </c>
       <c r="E127" t="s">
+        <v>334</v>
+      </c>
+      <c r="F127" t="s">
+        <v>335</v>
+      </c>
+      <c r="G127" t="s">
         <v>336</v>
       </c>
-      <c r="F127" t="s">
+      <c r="H127" t="s">
         <v>337</v>
-      </c>
-      <c r="G127" t="s">
-        <v>338</v>
-      </c>
-      <c r="H127" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B128" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C128" s="4">
         <v>0</v>
@@ -4357,24 +4357,24 @@
         <v>4</v>
       </c>
       <c r="E128" t="s">
+        <v>340</v>
+      </c>
+      <c r="F128" t="s">
+        <v>341</v>
+      </c>
+      <c r="G128" t="s">
         <v>342</v>
       </c>
-      <c r="F128" t="s">
+      <c r="H128" t="s">
         <v>343</v>
-      </c>
-      <c r="G128" t="s">
-        <v>344</v>
-      </c>
-      <c r="H128" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B129" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C129" s="4">
         <v>0</v>
@@ -4383,76 +4383,76 @@
         <v>2</v>
       </c>
       <c r="E129" t="s">
+        <v>346</v>
+      </c>
+      <c r="F129" t="s">
+        <v>347</v>
+      </c>
+      <c r="G129" t="s">
         <v>348</v>
       </c>
-      <c r="F129" t="s">
+      <c r="H129" t="s">
         <v>349</v>
-      </c>
-      <c r="G129" t="s">
-        <v>350</v>
-      </c>
-      <c r="H129" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>350</v>
+      </c>
+      <c r="B130" t="s">
+        <v>351</v>
+      </c>
+      <c r="C130" s="4">
+        <v>0</v>
+      </c>
+      <c r="D130" s="5">
+        <v>1</v>
+      </c>
+      <c r="E130" t="s">
         <v>352</v>
       </c>
-      <c r="B130" t="s">
+      <c r="F130" t="s">
         <v>353</v>
       </c>
-      <c r="C130" s="4">
-        <v>0</v>
-      </c>
-      <c r="D130" s="5">
-        <v>1</v>
-      </c>
-      <c r="E130" t="s">
+      <c r="G130" t="s">
         <v>354</v>
       </c>
-      <c r="F130" t="s">
+      <c r="H130" t="s">
         <v>355</v>
-      </c>
-      <c r="G130" t="s">
-        <v>356</v>
-      </c>
-      <c r="H130" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>356</v>
+      </c>
+      <c r="B131" t="s">
+        <v>357</v>
+      </c>
+      <c r="C131" s="4">
+        <v>0</v>
+      </c>
+      <c r="D131" s="5">
+        <v>1</v>
+      </c>
+      <c r="E131" t="s">
         <v>358</v>
       </c>
-      <c r="B131" t="s">
+      <c r="F131" t="s">
         <v>359</v>
       </c>
-      <c r="C131" s="4">
-        <v>0</v>
-      </c>
-      <c r="D131" s="5">
-        <v>1</v>
-      </c>
-      <c r="E131" t="s">
+      <c r="G131" t="s">
         <v>360</v>
       </c>
-      <c r="F131" t="s">
+      <c r="H131" t="s">
         <v>361</v>
-      </c>
-      <c r="G131" t="s">
-        <v>362</v>
-      </c>
-      <c r="H131" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B132" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C132" s="4">
         <v>0</v>
@@ -4461,79 +4461,79 @@
         <v>4</v>
       </c>
       <c r="F132" t="s">
+        <v>364</v>
+      </c>
+      <c r="G132" t="s">
+        <v>365</v>
+      </c>
+      <c r="H132" t="s">
         <v>366</v>
-      </c>
-      <c r="G132" t="s">
-        <v>367</v>
-      </c>
-      <c r="H132" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>367</v>
+      </c>
+      <c r="B133" t="s">
+        <v>368</v>
+      </c>
+      <c r="C133" s="4">
+        <v>0</v>
+      </c>
+      <c r="D133" s="5">
+        <v>1</v>
+      </c>
+      <c r="F133" t="s">
+        <v>364</v>
+      </c>
+      <c r="G133" t="s">
+        <v>365</v>
+      </c>
+      <c r="H133" t="s">
         <v>369</v>
-      </c>
-      <c r="B133" t="s">
-        <v>370</v>
-      </c>
-      <c r="C133" s="4">
-        <v>0</v>
-      </c>
-      <c r="D133" s="5">
-        <v>1</v>
-      </c>
-      <c r="F133" t="s">
-        <v>366</v>
-      </c>
-      <c r="G133" t="s">
-        <v>367</v>
-      </c>
-      <c r="H133" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>370</v>
+      </c>
+      <c r="B134" t="s">
+        <v>371</v>
+      </c>
+      <c r="C134" s="4">
+        <v>0</v>
+      </c>
+      <c r="D134" s="5">
+        <v>1</v>
+      </c>
+      <c r="E134" t="s">
         <v>372</v>
       </c>
-      <c r="B134" t="s">
+      <c r="F134" t="s">
         <v>373</v>
       </c>
-      <c r="C134" s="4">
-        <v>0</v>
-      </c>
-      <c r="D134" s="5">
-        <v>1</v>
-      </c>
-      <c r="E134" t="s">
+      <c r="G134" t="s">
         <v>374</v>
       </c>
-      <c r="F134" t="s">
+      <c r="H134" t="s">
         <v>375</v>
-      </c>
-      <c r="G134" t="s">
-        <v>376</v>
-      </c>
-      <c r="H134" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
+        <v>376</v>
+      </c>
+      <c r="B135" t="s">
+        <v>377</v>
+      </c>
+      <c r="C135" s="4">
+        <v>0</v>
+      </c>
+      <c r="D135" s="5">
+        <v>1</v>
+      </c>
+      <c r="E135" t="s">
         <v>378</v>
-      </c>
-      <c r="B135" t="s">
-        <v>379</v>
-      </c>
-      <c r="C135" s="4">
-        <v>0</v>
-      </c>
-      <c r="D135" s="5">
-        <v>1</v>
-      </c>
-      <c r="E135" t="s">
-        <v>380</v>
       </c>
       <c r="F135" t="s">
         <v>103</v>
@@ -4547,36 +4547,36 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>379</v>
+      </c>
+      <c r="B136" t="s">
+        <v>380</v>
+      </c>
+      <c r="C136" s="4">
+        <v>0</v>
+      </c>
+      <c r="D136" s="5">
+        <v>1</v>
+      </c>
+      <c r="E136" t="s">
         <v>381</v>
       </c>
-      <c r="B136" t="s">
+      <c r="F136" t="s">
         <v>382</v>
       </c>
-      <c r="C136" s="4">
-        <v>0</v>
-      </c>
-      <c r="D136" s="5">
-        <v>1</v>
-      </c>
-      <c r="E136" t="s">
+      <c r="G136" t="s">
         <v>383</v>
       </c>
-      <c r="F136" t="s">
+      <c r="H136" t="s">
         <v>384</v>
-      </c>
-      <c r="G136" t="s">
-        <v>385</v>
-      </c>
-      <c r="H136" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B137" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C137" s="4">
         <v>0</v>
@@ -4593,10 +4593,10 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B138" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C138" s="4">
         <v>0</v>
@@ -4610,10 +4610,10 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B139" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C139" s="4">
         <v>0</v>
@@ -4630,10 +4630,10 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B140" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C140" s="4">
         <v>0</v>
@@ -4650,10 +4650,10 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B141" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C141" s="4">
         <v>0</v>
@@ -4670,10 +4670,10 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B142" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C142" s="4">
         <v>0</v>
@@ -4690,10 +4690,10 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B143" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C143" s="4">
         <v>0</v>
@@ -4710,10 +4710,10 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B144" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C144" s="4">
         <v>0</v>
@@ -4730,10 +4730,10 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B145" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C145" s="4">
         <v>0</v>
@@ -4750,10 +4750,10 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B146" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C146" s="4">
         <v>0</v>
@@ -4770,10 +4770,10 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B147" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C147" s="4">
         <v>0</v>
@@ -4790,10 +4790,10 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B148" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C148" s="4">
         <v>0</v>
@@ -4810,10 +4810,10 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B149" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C149" s="4">
         <v>0</v>
@@ -4830,10 +4830,10 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B150" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C150" s="4">
         <v>0</v>
@@ -4867,10 +4867,10 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B152" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C152" s="4">
         <v>0</v>
@@ -4887,10 +4887,10 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B153" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C153" s="4">
         <v>0</v>
@@ -4907,10 +4907,10 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B154" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C154" s="4">
         <v>0</v>
@@ -4927,62 +4927,62 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
+        <v>419</v>
+      </c>
+      <c r="B155" t="s">
+        <v>438</v>
+      </c>
+      <c r="C155" s="4">
+        <v>0</v>
+      </c>
+      <c r="D155" s="5">
+        <v>1</v>
+      </c>
+      <c r="E155" t="s">
+        <v>420</v>
+      </c>
+      <c r="F155" t="s">
+        <v>321</v>
+      </c>
+      <c r="G155" t="s">
+        <v>322</v>
+      </c>
+      <c r="H155" t="s">
         <v>421</v>
-      </c>
-      <c r="B155" t="s">
-        <v>422</v>
-      </c>
-      <c r="C155" s="4">
-        <v>0</v>
-      </c>
-      <c r="D155" s="5">
-        <v>1</v>
-      </c>
-      <c r="E155" t="s">
-        <v>423</v>
-      </c>
-      <c r="F155" t="s">
-        <v>322</v>
-      </c>
-      <c r="G155" t="s">
-        <v>323</v>
-      </c>
-      <c r="H155" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
+        <v>422</v>
+      </c>
+      <c r="B156" t="s">
+        <v>423</v>
+      </c>
+      <c r="C156" s="4">
+        <v>0</v>
+      </c>
+      <c r="D156" s="5">
+        <v>1</v>
+      </c>
+      <c r="E156" t="s">
+        <v>424</v>
+      </c>
+      <c r="F156" t="s">
         <v>425</v>
       </c>
-      <c r="B156" t="s">
+      <c r="G156" t="s">
         <v>426</v>
       </c>
-      <c r="C156" s="4">
-        <v>0</v>
-      </c>
-      <c r="D156" s="5">
-        <v>1</v>
-      </c>
-      <c r="E156" t="s">
+      <c r="H156" t="s">
         <v>427</v>
-      </c>
-      <c r="F156" t="s">
-        <v>428</v>
-      </c>
-      <c r="G156" t="s">
-        <v>429</v>
-      </c>
-      <c r="H156" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B157" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C157" s="4">
         <v>0</v>
@@ -4991,7 +4991,7 @@
         <v>3</v>
       </c>
       <c r="F157" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="G157" t="s">
         <v>24</v>
@@ -4999,10 +4999,10 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B158" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C158" s="4">
         <v>0</v>
@@ -5011,21 +5011,21 @@
         <v>1</v>
       </c>
       <c r="F158" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="G158" t="s">
         <v>19</v>
       </c>
       <c r="H158" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B159" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C159" s="4">
         <v>0</v>
@@ -5034,7 +5034,7 @@
         <v>1</v>
       </c>
       <c r="F159" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="G159" t="s">
         <v>24</v>
@@ -5297,5 +5297,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FF53603-8F83-4C18-8DF4-CA00BEFBF0CD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FF53603-8F83-4C18-8DF4-CA00BEFBF0CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c8d62f16-0c2c-4704-a0dd-bcca6748d8b1"/>
+    <ds:schemaRef ds:uri="b03ebf58-9537-402b-8452-5979d44dca83"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>